<commit_message>
Update Week3 Day2 task and remove old Week1/Week2 files
</commit_message>
<xml_diff>
--- a/TASKS/Week3/Day2/Week3_Task_Day2.xlsx
+++ b/TASKS/Week3/Day2/Week3_Task_Day2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4b45fc5cd23d5b24/Documents/GIT/GenAI/TASKS/Week3/Day2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{04461C9A-AA72-4AA0-8A27-B8E662EE706B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EC90E8E-A721-4C2F-9A36-D4012DE52DEA}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{04461C9A-AA72-4AA0-8A27-B8E662EE706B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB7EA0E2-DE5B-452E-A26D-7D6B19D34E03}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{829622D8-041C-469B-BEAC-CA9616411F8F}"/>
+    <workbookView xWindow="1740" yWindow="1740" windowWidth="14400" windowHeight="8170" xr2:uid="{829622D8-041C-469B-BEAC-CA9616411F8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -175,7 +175,99 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>26028</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>6719</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAA9FD8B-22EA-22DA-9864-D6CE0F9159A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="14547850"/>
+          <a:ext cx="12218028" cy="7188569"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>26028</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>6719</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC7779FF-762F-6837-24BB-C4A8558354BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="21729700"/>
+          <a:ext cx="12218028" cy="7188569"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -497,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB6FB04-ADF6-4D0F-9ACD-9313AA147059}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>